<commit_message>
added new summary file
ALso added new summary file
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,6 +434,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Commute</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>wait_time</t>
@@ -497,50 +502,47 @@
       <c r="N1" s="1" t="inlineStr">
         <is>
           <t>avg_treat</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>avg_commute</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
       </c>
       <c r="B2" t="n">
         <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>249920</v>
+        <v>50460</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6591154931517644</v>
+        <v>0.74853024584738</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3217614272579343</v>
+        <v>0.3526294182996187</v>
       </c>
       <c r="F2" t="n">
-        <v>7.36486621867434</v>
+        <v>7.812576636820745</v>
       </c>
       <c r="G2" t="n">
-        <v>165.3492063492064</v>
+        <v>246.9</v>
       </c>
       <c r="H2" t="n">
-        <v>1355.31746031746</v>
+        <v>1518.5</v>
       </c>
       <c r="I2" t="n">
-        <v>2611.666666666667</v>
+        <v>3527.5</v>
       </c>
       <c r="J2" t="n">
-        <v>2633.206349206349</v>
+        <v>3789.3</v>
       </c>
       <c r="K2" t="n">
-        <v>1287.15873015873</v>
+        <v>1794.3</v>
       </c>
       <c r="L2" t="n">
-        <v>29291.23892181465</v>
+        <v>39524.4226115161</v>
       </c>
       <c r="M2" t="n">
         <v>1</v>
@@ -548,46 +550,45 @@
       <c r="N2" t="n">
         <v>0</v>
       </c>
-      <c r="O2" t="n">
-        <v>0.1587301587301587</v>
-      </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
       </c>
       <c r="B3" t="n">
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>244445</v>
+        <v>47241</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6242738562079848</v>
+        <v>0.733787678404157</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3489858641277275</v>
+        <v>0.3823043262558196</v>
       </c>
       <c r="F3" t="n">
-        <v>6.987457704534182</v>
+        <v>7.569324569233842</v>
       </c>
       <c r="G3" t="n">
-        <v>190.1269841269841</v>
+        <v>303.2</v>
       </c>
       <c r="H3" t="n">
-        <v>1460.698412698413</v>
+        <v>1539.9</v>
       </c>
       <c r="I3" t="n">
-        <v>2419.380952380952</v>
+        <v>3184.2</v>
       </c>
       <c r="J3" t="n">
-        <v>2438.301587301587</v>
+        <v>3474.4</v>
       </c>
       <c r="K3" t="n">
-        <v>1357.730158730159</v>
+        <v>1807.8</v>
       </c>
       <c r="L3" t="n">
-        <v>27183.20238974577</v>
+        <v>35744.22831054959</v>
       </c>
       <c r="M3" t="n">
         <v>1</v>
@@ -595,13 +596,12 @@
       <c r="N3" t="n">
         <v>1</v>
       </c>
-      <c r="O3" t="n">
-        <v>0.1587301587301587</v>
-      </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -609,34 +609,34 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-2.190701024327785</v>
+        <v>-6.379310344827586</v>
       </c>
       <c r="D4" t="n">
-        <v>-5.286120157360217</v>
+        <v>-1.969535302682866</v>
       </c>
       <c r="E4" t="n">
-        <v>8.461062937780071</v>
+        <v>8.415323967947291</v>
       </c>
       <c r="F4" t="n">
-        <v>-5.12444493809272</v>
+        <v>-3.113595922252512</v>
       </c>
       <c r="G4" t="n">
-        <v>14.98512047614476</v>
+        <v>22.80275415147833</v>
       </c>
       <c r="H4" t="n">
-        <v>7.775370381214509</v>
+        <v>1.409285479091215</v>
       </c>
       <c r="I4" t="n">
-        <v>-7.362567234934813</v>
+        <v>-9.732104890148836</v>
       </c>
       <c r="J4" t="n">
-        <v>-7.401803583054035</v>
+        <v>-8.310241997202651</v>
       </c>
       <c r="K4" t="n">
-        <v>5.482729279451489</v>
+        <v>0.7523825447249624</v>
       </c>
       <c r="L4" t="n">
-        <v>-7.196815872813479</v>
+        <v>-9.564198668053633</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
@@ -646,8 +646,147 @@
           <t>inf</t>
         </is>
       </c>
-      <c r="O4" t="n">
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="n">
+        <v>199460</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.6422447850959879</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.3159372780047863</v>
+      </c>
+      <c r="F5" t="n">
+        <v>7.280392554873131</v>
+      </c>
+      <c r="G5" t="n">
+        <v>149.9622641509434</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1324.528301886792</v>
+      </c>
+      <c r="I5" t="n">
+        <v>2438.867924528302</v>
+      </c>
+      <c r="J5" t="n">
+        <v>2415.075471698113</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1191.471698113208</v>
+      </c>
+      <c r="L5" t="n">
+        <v>27360.44954639928</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>197204</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.6036108708879523</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.3426993618394082</v>
+      </c>
+      <c r="F6" t="n">
+        <v>6.877671503647454</v>
+      </c>
+      <c r="G6" t="n">
+        <v>168.7924528301887</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1445.754716981132</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2275.075471698113</v>
+      </c>
+      <c r="J6" t="n">
+        <v>2242.811320754717</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1272.811320754717</v>
+      </c>
+      <c r="L6" t="n">
+        <v>25567.91448016014</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Difference (%)</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>-1.131053845382533</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-6.01545004406093</v>
+      </c>
+      <c r="E7" t="n">
+        <v>8.4706951973602</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-5.53158429563137</v>
+      </c>
+      <c r="G7" t="n">
+        <v>12.55661801711122</v>
+      </c>
+      <c r="H7" t="n">
+        <v>9.152421652421658</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-6.715921398731241</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-7.132868225533007</v>
+      </c>
+      <c r="K7" t="n">
+        <v>6.826819535060483</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-6.5515556065673</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed total shared rides to avg
Changed the total shared rides to average.
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -446,7 +446,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>total_shared_rides</t>
+          <t>avg_shared_rides</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -515,7 +515,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>50460</v>
+        <v>5046</v>
       </c>
       <c r="D2" t="n">
         <v>0.74853024584738</v>
@@ -561,7 +561,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>47241</v>
+        <v>4724.1</v>
       </c>
       <c r="D3" t="n">
         <v>0.733787678404157</v>
@@ -609,7 +609,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-6.379310344827586</v>
+        <v>-6.379310344827579</v>
       </c>
       <c r="D4" t="n">
         <v>-1.969535302682866</v>
@@ -657,7 +657,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>199460</v>
+        <v>3763.396226415094</v>
       </c>
       <c r="D5" t="n">
         <v>0.6422447850959879</v>
@@ -703,7 +703,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>197204</v>
+        <v>3720.830188679245</v>
       </c>
       <c r="D6" t="n">
         <v>0.6036108708879523</v>
@@ -751,7 +751,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-1.131053845382533</v>
+        <v>-1.131053845382532</v>
       </c>
       <c r="D7" t="n">
         <v>-6.01545004406093</v>

</xml_diff>